<commit_message>
Changed testing files from XML spreadsheet to Excel workbook.
</commit_message>
<xml_diff>
--- a/Testing_data/AdductList.xlsx
+++ b/Testing_data/AdductList.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/River/Desktop/RTP/xlxs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/River/Desktop/Coding/QT/RTP_QT/Testing_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6541A6DA-5B28-0C48-8AFE-9B9EC07E06F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53012000-BF7D-B746-A2A5-449EA5DE8BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="1960" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="10360" yWindow="1960" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdductList" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Structure</t>
   </si>
@@ -54,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -374,15 +369,15 @@
   </fills>
   <borders count="10">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -390,8 +385,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -399,8 +394,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -408,12 +403,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF7F7F7F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -423,12 +418,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -438,8 +433,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -447,12 +442,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="double">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="double">
+      </left>
+      <right style="double">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -462,12 +457,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FFB2B2B2"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -477,8 +472,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -593,7 +588,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -746,25 +741,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -772,25 +767,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -803,21 +798,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -831,7 +826,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -843,32 +838,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -888,7 +883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>